<commit_message>
More exploratory analysis Corrected bad equation in excel sheet
</commit_message>
<xml_diff>
--- a/SYE data sheet.xlsx
+++ b/SYE data sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claramugnai/Desktop/Fall 2021/SYE/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD468E9D-425C-4A46-9971-FE437D1594FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC59E34-4175-B54A-ACA2-9616B1C431CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" xr2:uid="{6BEEF0CC-3BFA-F34B-B6A4-F2A8386DF928}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770BFC5D-9962-BA42-A40D-DF7A3C038E19}">
   <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,10 +974,12 @@
         <v>0</v>
       </c>
       <c r="T2">
+        <f>SUM(L2,Q2,S2)</f>
         <v>20</v>
       </c>
       <c r="U2">
-        <v>19</v>
+        <f>SUM(M2,N2,O2,P2,R2)</f>
+        <v>15</v>
       </c>
       <c r="V2">
         <v>1</v>
@@ -1040,10 +1042,12 @@
         <v>0</v>
       </c>
       <c r="T3">
+        <f t="shared" ref="T3:T11" si="0">SUM(L3,Q3,S3)</f>
         <v>28</v>
       </c>
       <c r="U3">
-        <v>8</v>
+        <f t="shared" ref="U3:U60" si="1">SUM(M3,N3,O3,P3,R3)</f>
+        <v>6</v>
       </c>
       <c r="V3">
         <v>20</v>
@@ -1106,9 +1110,11 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="U4">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="V4">
@@ -1171,9 +1177,11 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="U5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V5">
@@ -1236,9 +1244,11 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="U6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V6">
@@ -1298,9 +1308,11 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="U7">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V7">
@@ -1360,9 +1372,11 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="U8">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V8">
@@ -1422,9 +1436,11 @@
         <v>8</v>
       </c>
       <c r="T9">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="U9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V9">
@@ -1487,10 +1503,12 @@
         <v>0</v>
       </c>
       <c r="T10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U10">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="V10">
         <v>12</v>
@@ -1552,12 +1570,12 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <f>SUM(K11,P11,R11)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="U11">
-        <f>SUM(L11,M11,N11,O11,Q11)</f>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="V11">
         <v>30</v>
@@ -1619,12 +1637,12 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12:T58" si="0">SUM(K12,P12,R12)</f>
-        <v>0</v>
+        <f>SUM(L12,Q12,S12)</f>
+        <v>31</v>
       </c>
       <c r="U12">
-        <f t="shared" ref="U12:U58" si="1">SUM(L12,M12,N12,O12,Q12)</f>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="V12">
         <v>29</v>
@@ -1683,12 +1701,12 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="T13:T60" si="2">SUM(L13,Q13,S13)</f>
+        <v>33</v>
       </c>
       <c r="U13">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="V13">
         <v>29</v>
@@ -1750,12 +1768,12 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U14">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <v>32</v>
@@ -1817,12 +1835,12 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="U15">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="V15">
         <v>23</v>
@@ -1881,12 +1899,12 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U16">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V16">
         <v>32</v>
@@ -1951,12 +1969,12 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="U17">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>33</v>
@@ -2015,12 +2033,12 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="U18">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <v>31</v>
@@ -2082,12 +2100,12 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="U19">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="V19">
         <v>18</v>
@@ -2146,12 +2164,12 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U20">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V20">
         <v>34</v>
@@ -2210,12 +2228,12 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="U21">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="V21">
         <v>32</v>
@@ -2277,12 +2295,12 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="U22">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="V22">
         <v>-4</v>
@@ -2341,12 +2359,12 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="U23">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="V23">
         <v>19</v>
@@ -2408,12 +2426,12 @@
         <v>0</v>
       </c>
       <c r="T24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="U24">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="V24">
         <v>32</v>
@@ -2475,12 +2493,12 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="U25">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="V25">
         <v>16</v>
@@ -2539,12 +2557,12 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="U26">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="V26">
         <v>28</v>
@@ -2603,12 +2621,12 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="U27">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="V27">
         <v>18</v>
@@ -2667,12 +2685,12 @@
         <v>10</v>
       </c>
       <c r="T28">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U28">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V28">
         <v>32</v>
@@ -2731,12 +2749,12 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U29">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V29">
         <v>34</v>
@@ -2798,12 +2816,12 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="U30">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="V30">
         <v>15</v>
@@ -2865,12 +2883,12 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="U31">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="V31">
         <v>5</v>
@@ -2935,12 +2953,12 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="U32">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="V32">
         <v>23</v>
@@ -2999,12 +3017,12 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="U33">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="V33">
         <v>23</v>
@@ -3066,12 +3084,12 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U34">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <v>34</v>
@@ -3133,12 +3151,12 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U35">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V35">
         <v>34</v>
@@ -3197,12 +3215,12 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U36">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V36">
         <v>34</v>
@@ -3261,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U37">
@@ -3328,12 +3346,12 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="U38">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="V38">
         <v>21</v>
@@ -3395,12 +3413,12 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="U39">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="V39">
         <v>20</v>
@@ -3462,12 +3480,12 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="U40">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="V40">
         <v>19</v>
@@ -3526,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U41">
@@ -3593,12 +3611,12 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="U42">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="V42">
         <v>12</v>
@@ -3657,12 +3675,12 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="U43">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="V43">
         <v>-16</v>
@@ -3724,12 +3742,12 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U44">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V44">
         <v>32</v>
@@ -3785,12 +3803,12 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="U45">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="V45">
         <v>23</v>
@@ -3846,12 +3864,12 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="U46">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="V46">
         <v>21</v>
@@ -3907,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U47">
@@ -3971,12 +3989,12 @@
         <v>0</v>
       </c>
       <c r="T48">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="U48">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="V48">
         <v>19</v>
@@ -4035,12 +4053,12 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U49">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V49">
         <v>32</v>
@@ -4102,12 +4120,12 @@
         <v>0</v>
       </c>
       <c r="T50">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="U50">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="V50">
         <v>6</v>
@@ -4169,12 +4187,12 @@
         <v>0</v>
       </c>
       <c r="T51">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="U51">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="V51">
         <v>3</v>
@@ -4233,12 +4251,12 @@
         <v>0</v>
       </c>
       <c r="T52">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="U52">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="V52">
         <v>7</v>
@@ -4297,12 +4315,12 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="U53">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="V53">
         <v>4</v>
@@ -4358,12 +4376,12 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U54">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V54">
         <v>34</v>
@@ -4419,12 +4437,12 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="U55">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="V55">
         <v>24</v>
@@ -4480,12 +4498,12 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="U56">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="V56">
         <v>20</v>
@@ -4541,12 +4559,12 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="U57">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="V57">
         <v>34</v>
@@ -4602,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U58">
@@ -4663,12 +4681,12 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <f t="shared" ref="T59:T60" si="2">SUM(K59,P59,R59)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="U59">
-        <f t="shared" ref="U59:U60" si="3">SUM(L59,M59,N59,O59,Q59)</f>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -4728,7 +4746,7 @@
         <v>0</v>
       </c>
       <c r="U60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="V60">

</xml_diff>

<commit_message>
Attempted to finish fixing the time issue, edited the excel sheet to fix am/pm, encountered issues with shiny output.
</commit_message>
<xml_diff>
--- a/SYE data sheet.xlsx
+++ b/SYE data sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claramugnai/Desktop/Fall 2021/SYE/Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claramugnai/Desktop/Spring 2022/SYE/SYE_spring2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC59E34-4175-B54A-ACA2-9616B1C431CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A65AA3-1041-CB47-8465-97833A80949F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" xr2:uid="{6BEEF0CC-3BFA-F34B-B6A4-F2A8386DF928}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="144">
   <si>
     <t>Horse</t>
   </si>
@@ -414,6 +414,60 @@
   </si>
   <si>
     <t>Huntfield</t>
+  </si>
+  <si>
+    <t>A.M./P.M.</t>
+  </si>
+  <si>
+    <t>10-10:30</t>
+  </si>
+  <si>
+    <t>a.m.</t>
+  </si>
+  <si>
+    <t>11:30-12</t>
+  </si>
+  <si>
+    <t>7:30-8</t>
+  </si>
+  <si>
+    <t>p.m.</t>
+  </si>
+  <si>
+    <t>7-7:30</t>
+  </si>
+  <si>
+    <t>11-11:30</t>
+  </si>
+  <si>
+    <t>9-9:30</t>
+  </si>
+  <si>
+    <t>10:30-11</t>
+  </si>
+  <si>
+    <t>9:30-10</t>
+  </si>
+  <si>
+    <t>6:30-7</t>
+  </si>
+  <si>
+    <t>12-12:30</t>
+  </si>
+  <si>
+    <t>5:30-6</t>
+  </si>
+  <si>
+    <t>1-1:30</t>
+  </si>
+  <si>
+    <t>1:30-2</t>
+  </si>
+  <si>
+    <t>2-2:30</t>
+  </si>
+  <si>
+    <t>3-3:30</t>
   </si>
 </sst>
 </file>
@@ -843,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770BFC5D-9962-BA42-A40D-DF7A3C038E19}">
   <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="Q42" workbookViewId="0">
+      <selection activeCell="W61" sqref="W61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,6 +970,9 @@
       <c r="V1" t="s">
         <v>15</v>
       </c>
+      <c r="W1" t="s">
+        <v>126</v>
+      </c>
       <c r="AA1" s="13"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -926,7 +983,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D2" s="12">
         <v>24</v>
@@ -984,6 +1041,9 @@
       <c r="V2">
         <v>1</v>
       </c>
+      <c r="W2" t="s">
+        <v>128</v>
+      </c>
       <c r="AA2" s="14"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -994,7 +1054,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D3" s="12">
         <v>12</v>
@@ -1052,6 +1112,9 @@
       <c r="V3">
         <v>20</v>
       </c>
+      <c r="W3" t="s">
+        <v>128</v>
+      </c>
       <c r="AA3" s="15"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -1062,7 +1125,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D4" s="12">
         <v>5</v>
@@ -1120,6 +1183,9 @@
       <c r="V4">
         <v>10</v>
       </c>
+      <c r="W4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -1129,7 +1195,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="D5" s="12">
         <v>9</v>
@@ -1187,6 +1253,9 @@
       <c r="V5">
         <v>34</v>
       </c>
+      <c r="W5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
@@ -1196,7 +1265,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="D6" s="12">
         <v>12</v>
@@ -1254,6 +1323,9 @@
       <c r="V6">
         <v>34</v>
       </c>
+      <c r="W6" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1263,7 +1335,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="D7" s="12">
         <v>25</v>
@@ -1318,6 +1390,9 @@
       <c r="V7">
         <v>33</v>
       </c>
+      <c r="W7" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -1327,7 +1402,7 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="D8" s="12">
         <v>17</v>
@@ -1381,6 +1456,9 @@
       </c>
       <c r="V8">
         <v>31</v>
+      </c>
+      <c r="W8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -1391,7 +1469,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="D9" s="12">
         <v>10</v>
@@ -1445,6 +1523,9 @@
       </c>
       <c r="V9">
         <v>34</v>
+      </c>
+      <c r="W9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -1455,7 +1536,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D10" s="12">
         <v>24</v>
@@ -1513,6 +1594,9 @@
       <c r="V10">
         <v>12</v>
       </c>
+      <c r="W10" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
@@ -1522,7 +1606,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D11" s="12">
         <v>9</v>
@@ -1580,6 +1664,9 @@
       <c r="V11">
         <v>30</v>
       </c>
+      <c r="W11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
@@ -1589,7 +1676,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D12" s="12">
         <v>12</v>
@@ -1647,6 +1734,9 @@
       <c r="V12">
         <v>29</v>
       </c>
+      <c r="W12" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
@@ -1656,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D13" s="12">
         <v>25</v>
@@ -1711,6 +1801,9 @@
       <c r="V13">
         <v>29</v>
       </c>
+      <c r="W13" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -1720,7 +1813,7 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D14" s="12">
         <v>22</v>
@@ -1777,6 +1870,9 @@
       </c>
       <c r="V14">
         <v>32</v>
+      </c>
+      <c r="W14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
@@ -1787,7 +1883,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D15" s="12">
         <v>24</v>
@@ -1845,6 +1941,9 @@
       <c r="V15">
         <v>23</v>
       </c>
+      <c r="W15" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1854,7 +1953,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D16" s="12">
         <v>18</v>
@@ -1909,8 +2008,11 @@
       <c r="V16">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
@@ -1918,7 +2020,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="D17" s="12">
         <v>22</v>
@@ -1979,8 +2081,11 @@
       <c r="V17">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>42</v>
       </c>
@@ -1988,7 +2093,7 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="D18" s="12">
         <v>28</v>
@@ -2043,8 +2148,11 @@
       <c r="V18">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
@@ -2052,7 +2160,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D19" s="12">
         <v>24</v>
@@ -2110,8 +2218,11 @@
       <c r="V19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -2119,7 +2230,7 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D20" s="12">
         <v>17</v>
@@ -2174,8 +2285,11 @@
       <c r="V20">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -2183,7 +2297,7 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D21" s="12">
         <v>10</v>
@@ -2238,8 +2352,11 @@
       <c r="V21">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>17</v>
       </c>
@@ -2247,7 +2364,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
@@ -2305,8 +2422,11 @@
       <c r="V22">
         <v>-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>44</v>
       </c>
@@ -2314,7 +2434,7 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="D23" s="12">
         <v>12</v>
@@ -2369,8 +2489,11 @@
       <c r="V23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>10</v>
       </c>
@@ -2378,7 +2501,7 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D24" s="12">
         <v>12</v>
@@ -2436,8 +2559,11 @@
       <c r="V24">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
@@ -2445,7 +2571,7 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D25" s="12">
         <v>19</v>
@@ -2503,8 +2629,11 @@
       <c r="V25">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
@@ -2512,7 +2641,7 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D26" s="12">
         <v>19</v>
@@ -2567,8 +2696,11 @@
       <c r="V26">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
@@ -2576,7 +2708,7 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D27" s="12">
         <v>12</v>
@@ -2631,8 +2763,11 @@
       <c r="V27">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -2640,7 +2775,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D28" s="12">
         <v>24</v>
@@ -2695,8 +2830,11 @@
       <c r="V28">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
@@ -2704,7 +2842,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D29" s="12">
         <v>18</v>
@@ -2759,8 +2897,11 @@
       <c r="V29">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>44</v>
       </c>
@@ -2768,7 +2909,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D30" s="12">
         <v>12</v>
@@ -2826,8 +2967,11 @@
       <c r="V30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
@@ -2835,7 +2979,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D31" s="12">
         <v>5</v>
@@ -2893,8 +3037,11 @@
       <c r="V31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -2902,7 +3049,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="D32" s="12">
         <v>22</v>
@@ -2963,8 +3110,11 @@
       <c r="V32">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -2972,7 +3122,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="D33" s="12">
         <v>28</v>
@@ -3027,8 +3177,11 @@
       <c r="V33">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>21</v>
       </c>
@@ -3036,7 +3189,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D34" s="12">
         <v>9</v>
@@ -3094,8 +3247,11 @@
       <c r="V34">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>22</v>
       </c>
@@ -3103,7 +3259,7 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D35" s="12">
         <v>12</v>
@@ -3161,8 +3317,11 @@
       <c r="V35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
@@ -3170,7 +3329,7 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D36" s="12">
         <v>25</v>
@@ -3225,8 +3384,11 @@
       <c r="V36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>35</v>
       </c>
@@ -3234,7 +3396,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="D37" s="12">
         <v>22</v>
@@ -3289,8 +3451,11 @@
       <c r="V37">
         <v>-11</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>49</v>
       </c>
@@ -3298,7 +3463,7 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D38" s="12">
         <v>15</v>
@@ -3356,8 +3521,11 @@
       <c r="V38">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>50</v>
       </c>
@@ -3365,7 +3533,7 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D39" s="12">
         <v>14</v>
@@ -3423,8 +3591,11 @@
       <c r="V39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>45</v>
       </c>
@@ -3432,7 +3603,7 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="D40" s="12">
         <v>19</v>
@@ -3490,8 +3661,11 @@
       <c r="V40">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>52</v>
       </c>
@@ -3499,7 +3673,7 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="D41" s="12">
         <v>18</v>
@@ -3554,8 +3728,11 @@
       <c r="V41">
         <v>-13</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>53</v>
       </c>
@@ -3563,7 +3740,7 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D42" s="12">
         <v>19</v>
@@ -3621,8 +3798,11 @@
       <c r="V42">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>52</v>
       </c>
@@ -3630,7 +3810,7 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D43" s="12">
         <v>18</v>
@@ -3685,8 +3865,11 @@
       <c r="V43">
         <v>-16</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>35</v>
       </c>
@@ -3694,7 +3877,7 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="D44" s="12">
         <v>22</v>
@@ -3752,8 +3935,11 @@
       <c r="V44">
         <v>32</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>26</v>
       </c>
@@ -3761,7 +3947,7 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D45" s="12">
         <v>17</v>
@@ -3813,8 +3999,11 @@
       <c r="V45">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>27</v>
       </c>
@@ -3822,7 +4011,7 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D46" s="12">
         <v>10</v>
@@ -3874,8 +4063,11 @@
       <c r="V46">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>52</v>
       </c>
@@ -3883,7 +4075,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D47" s="12">
         <v>18</v>
@@ -3935,8 +4127,11 @@
       <c r="V47">
         <v>-32</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>39</v>
       </c>
@@ -3944,7 +4139,7 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="D48" s="12">
         <v>24</v>
@@ -3999,8 +4194,11 @@
       <c r="V48">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>37</v>
       </c>
@@ -4008,7 +4206,7 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="D49" s="12">
         <v>18</v>
@@ -4063,8 +4261,11 @@
       <c r="V49">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>49</v>
       </c>
@@ -4072,7 +4273,7 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D50" s="12">
         <v>15</v>
@@ -4130,8 +4331,11 @@
       <c r="V50">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>50</v>
       </c>
@@ -4139,7 +4343,7 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D51" s="12">
         <v>14</v>
@@ -4197,8 +4401,11 @@
       <c r="V51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>49</v>
       </c>
@@ -4206,7 +4413,7 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D52" s="12">
         <v>15</v>
@@ -4261,8 +4468,11 @@
       <c r="V52">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>50</v>
       </c>
@@ -4270,7 +4480,7 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D53" s="12">
         <v>14</v>
@@ -4325,8 +4535,11 @@
       <c r="V53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>37</v>
       </c>
@@ -4334,7 +4547,7 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D54" s="12">
         <v>18</v>
@@ -4386,8 +4599,11 @@
       <c r="V54">
         <v>34</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>39</v>
       </c>
@@ -4395,7 +4611,7 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D55" s="12">
         <v>24</v>
@@ -4447,8 +4663,11 @@
       <c r="V55">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>39</v>
       </c>
@@ -4456,7 +4675,7 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D56" s="12">
         <v>24</v>
@@ -4508,8 +4727,11 @@
       <c r="V56">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W56" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>37</v>
       </c>
@@ -4517,7 +4739,7 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D57" s="12">
         <v>18</v>
@@ -4569,8 +4791,11 @@
       <c r="V57">
         <v>34</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>41</v>
       </c>
@@ -4578,7 +4803,7 @@
         <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D58" s="12">
         <v>22</v>
@@ -4630,8 +4855,11 @@
       <c r="V58">
         <v>-6</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>42</v>
       </c>
@@ -4639,7 +4867,7 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D59" s="12">
         <v>28</v>
@@ -4691,8 +4919,11 @@
       <c r="V59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>44</v>
       </c>
@@ -4700,7 +4931,7 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D60" s="12">
         <v>12</v>
@@ -4751,6 +4982,9 @@
       </c>
       <c r="V60">
         <v>-4</v>
+      </c>
+      <c r="W60" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shiny app completed - not sure what next step is. The html output and the app complement each other well
</commit_message>
<xml_diff>
--- a/SYE data sheet.xlsx
+++ b/SYE data sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claramugnai/Desktop/Spring 2022/SYE/SYE_spring2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A65AA3-1041-CB47-8465-97833A80949F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE23680-2F56-E841-8036-7E0BA73A2CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" xr2:uid="{6BEEF0CC-3BFA-F34B-B6A4-F2A8386DF928}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="128">
   <si>
     <t>Horse</t>
   </si>
@@ -416,65 +416,17 @@
     <t>Huntfield</t>
   </si>
   <si>
-    <t>A.M./P.M.</t>
-  </si>
-  <si>
-    <t>10-10:30</t>
-  </si>
-  <si>
-    <t>a.m.</t>
-  </si>
-  <si>
-    <t>11:30-12</t>
-  </si>
-  <si>
-    <t>7:30-8</t>
-  </si>
-  <si>
-    <t>p.m.</t>
-  </si>
-  <si>
-    <t>7-7:30</t>
-  </si>
-  <si>
-    <t>11-11:30</t>
-  </si>
-  <si>
-    <t>9-9:30</t>
-  </si>
-  <si>
-    <t>10:30-11</t>
-  </si>
-  <si>
-    <t>9:30-10</t>
-  </si>
-  <si>
-    <t>6:30-7</t>
-  </si>
-  <si>
-    <t>12-12:30</t>
-  </si>
-  <si>
-    <t>5:30-6</t>
-  </si>
-  <si>
-    <t>1-1:30</t>
-  </si>
-  <si>
-    <t>1:30-2</t>
-  </si>
-  <si>
-    <t>2-2:30</t>
-  </si>
-  <si>
-    <t>3-3:30</t>
+    <t>Start_time</t>
+  </si>
+  <si>
+    <t>End_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,6 +458,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,13 +515,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -578,10 +539,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -895,23 +858,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770BFC5D-9962-BA42-A40D-DF7A3C038E19}">
-  <dimension ref="A1:AA60"/>
+  <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q42" workbookViewId="0">
-      <selection activeCell="W61" sqref="W61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -970,20 +933,17 @@
       <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA1" s="13"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>127</v>
+      <c r="B2" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.4375</v>
       </c>
       <c r="D2" s="12">
         <v>24</v>
@@ -1041,20 +1001,17 @@
       <c r="V2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA2" s="14"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y2" s="14"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>127</v>
+      <c r="B3" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.4375</v>
       </c>
       <c r="D3" s="12">
         <v>12</v>
@@ -1112,20 +1069,17 @@
       <c r="V3">
         <v>20</v>
       </c>
-      <c r="W3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA3" s="15"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>129</v>
+      <c r="B4" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
       </c>
       <c r="D4" s="12">
         <v>5</v>
@@ -1183,19 +1137,16 @@
       <c r="V4">
         <v>10</v>
       </c>
-      <c r="W4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
+      <c r="B5" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D5" s="12">
         <v>9</v>
@@ -1253,19 +1204,16 @@
       <c r="V5">
         <v>34</v>
       </c>
-      <c r="W5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
+      <c r="B6" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D6" s="12">
         <v>12</v>
@@ -1323,19 +1271,16 @@
       <c r="V6">
         <v>34</v>
       </c>
-      <c r="W6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>130</v>
+      <c r="B7" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D7" s="12">
         <v>25</v>
@@ -1390,19 +1335,16 @@
       <c r="V7">
         <v>33</v>
       </c>
-      <c r="W7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>132</v>
+      <c r="B8" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.3125</v>
       </c>
       <c r="D8" s="12">
         <v>17</v>
@@ -1457,19 +1399,16 @@
       <c r="V8">
         <v>31</v>
       </c>
-      <c r="W8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>132</v>
+      <c r="B9" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.3125</v>
       </c>
       <c r="D9" s="12">
         <v>10</v>
@@ -1524,19 +1463,16 @@
       <c r="V9">
         <v>34</v>
       </c>
-      <c r="W9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>133</v>
+      <c r="B10" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.47916666666666669</v>
       </c>
       <c r="D10" s="12">
         <v>24</v>
@@ -1594,19 +1530,16 @@
       <c r="V10">
         <v>12</v>
       </c>
-      <c r="W10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
+      <c r="B11" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="D11" s="12">
         <v>9</v>
@@ -1664,19 +1597,16 @@
       <c r="V11">
         <v>30</v>
       </c>
-      <c r="W11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
+      <c r="B12" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="D12" s="12">
         <v>12</v>
@@ -1734,19 +1664,16 @@
       <c r="V12">
         <v>29</v>
       </c>
-      <c r="W12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>130</v>
+      <c r="B13" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="D13" s="12">
         <v>25</v>
@@ -1801,19 +1728,16 @@
       <c r="V13">
         <v>29</v>
       </c>
-      <c r="W13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B14">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>127</v>
+      <c r="B14" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.4375</v>
       </c>
       <c r="D14" s="12">
         <v>22</v>
@@ -1871,19 +1795,16 @@
       <c r="V14">
         <v>32</v>
       </c>
-      <c r="W14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B15">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>134</v>
+      <c r="B15" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.39583333333333331</v>
       </c>
       <c r="D15" s="12">
         <v>24</v>
@@ -1941,19 +1862,16 @@
       <c r="V15">
         <v>23</v>
       </c>
-      <c r="W15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B16">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>134</v>
+      <c r="B16" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.39583333333333331</v>
       </c>
       <c r="D16" s="12">
         <v>18</v>
@@ -2008,19 +1926,16 @@
       <c r="V16">
         <v>32</v>
       </c>
-      <c r="W16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B17">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>135</v>
+      <c r="B17" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.45833333333333331</v>
       </c>
       <c r="D17" s="12">
         <v>22</v>
@@ -2081,19 +1996,16 @@
       <c r="V17">
         <v>33</v>
       </c>
-      <c r="W17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B18">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>135</v>
+      <c r="B18" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.45833333333333331</v>
       </c>
       <c r="D18" s="12">
         <v>28</v>
@@ -2148,19 +2060,16 @@
       <c r="V18">
         <v>31</v>
       </c>
-      <c r="W18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B19">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>136</v>
+      <c r="B19" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.41666666666666669</v>
       </c>
       <c r="D19" s="12">
         <v>24</v>
@@ -2218,19 +2127,16 @@
       <c r="V19">
         <v>18</v>
       </c>
-      <c r="W19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B20">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>137</v>
+      <c r="B20" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D20" s="12">
         <v>17</v>
@@ -2285,19 +2191,16 @@
       <c r="V20">
         <v>34</v>
       </c>
-      <c r="W20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>137</v>
+      <c r="B21" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D21" s="12">
         <v>10</v>
@@ -2352,19 +2255,16 @@
       <c r="V21">
         <v>32</v>
       </c>
-      <c r="W21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B22">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>132</v>
+      <c r="B22" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.3125</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
@@ -2422,19 +2322,16 @@
       <c r="V22">
         <v>-4</v>
       </c>
-      <c r="W22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B23">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>132</v>
+      <c r="B23" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.3125</v>
       </c>
       <c r="D23" s="12">
         <v>12</v>
@@ -2489,19 +2386,16 @@
       <c r="V23">
         <v>19</v>
       </c>
-      <c r="W23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B24">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>129</v>
+      <c r="B24" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.5</v>
       </c>
       <c r="D24" s="12">
         <v>12</v>
@@ -2559,19 +2453,16 @@
       <c r="V24">
         <v>32</v>
       </c>
-      <c r="W24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B25">
-        <v>30</v>
-      </c>
-      <c r="C25" t="s">
-        <v>129</v>
+      <c r="B25" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.5</v>
       </c>
       <c r="D25" s="12">
         <v>19</v>
@@ -2629,19 +2520,16 @@
       <c r="V25">
         <v>16</v>
       </c>
-      <c r="W25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>127</v>
+      <c r="B26" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.4375</v>
       </c>
       <c r="D26" s="12">
         <v>19</v>
@@ -2696,19 +2584,16 @@
       <c r="V26">
         <v>28</v>
       </c>
-      <c r="W26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B27">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>127</v>
+      <c r="B27" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.4375</v>
       </c>
       <c r="D27" s="12">
         <v>12</v>
@@ -2763,19 +2648,16 @@
       <c r="V27">
         <v>18</v>
       </c>
-      <c r="W27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B28">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>129</v>
+      <c r="B28" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.5</v>
       </c>
       <c r="D28" s="12">
         <v>24</v>
@@ -2830,19 +2712,16 @@
       <c r="V28">
         <v>32</v>
       </c>
-      <c r="W28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B29">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>129</v>
+      <c r="B29" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.5</v>
       </c>
       <c r="D29" s="12">
         <v>18</v>
@@ -2897,19 +2776,16 @@
       <c r="V29">
         <v>34</v>
       </c>
-      <c r="W29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B30">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>137</v>
+      <c r="B30" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D30" s="12">
         <v>12</v>
@@ -2967,19 +2843,16 @@
       <c r="V30">
         <v>15</v>
       </c>
-      <c r="W30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>137</v>
+      <c r="B31" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D31" s="12">
         <v>5</v>
@@ -3037,19 +2910,16 @@
       <c r="V31">
         <v>5</v>
       </c>
-      <c r="W31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B32">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>138</v>
+      <c r="B32" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.52083333333333337</v>
       </c>
       <c r="D32" s="12">
         <v>22</v>
@@ -3110,19 +2980,16 @@
       <c r="V32">
         <v>23</v>
       </c>
-      <c r="W32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B33">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>138</v>
+      <c r="B33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.52083333333333337</v>
       </c>
       <c r="D33" s="12">
         <v>28</v>
@@ -3177,19 +3044,16 @@
       <c r="V33">
         <v>23</v>
       </c>
-      <c r="W33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B34">
-        <v>30</v>
-      </c>
-      <c r="C34" t="s">
-        <v>139</v>
+      <c r="B34" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.75</v>
       </c>
       <c r="D34" s="12">
         <v>9</v>
@@ -3247,19 +3111,16 @@
       <c r="V34">
         <v>34</v>
       </c>
-      <c r="W34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B35">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
-        <v>139</v>
+      <c r="B35" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.75</v>
       </c>
       <c r="D35" s="12">
         <v>12</v>
@@ -3317,19 +3178,16 @@
       <c r="V35">
         <v>34</v>
       </c>
-      <c r="W35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B36">
-        <v>30</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
+      <c r="B36" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.75</v>
       </c>
       <c r="D36" s="12">
         <v>25</v>
@@ -3384,19 +3242,16 @@
       <c r="V36">
         <v>34</v>
       </c>
-      <c r="W36" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>30</v>
-      </c>
-      <c r="C37" t="s">
-        <v>140</v>
+      <c r="B37" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.5625</v>
       </c>
       <c r="D37" s="12">
         <v>22</v>
@@ -3451,19 +3306,16 @@
       <c r="V37">
         <v>-11</v>
       </c>
-      <c r="W37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B38">
-        <v>30</v>
-      </c>
-      <c r="C38" t="s">
-        <v>129</v>
+      <c r="B38" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.5</v>
       </c>
       <c r="D38" s="12">
         <v>15</v>
@@ -3521,19 +3373,16 @@
       <c r="V38">
         <v>21</v>
       </c>
-      <c r="W38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B39">
-        <v>30</v>
-      </c>
-      <c r="C39" t="s">
-        <v>129</v>
+      <c r="B39" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.5</v>
       </c>
       <c r="D39" s="12">
         <v>14</v>
@@ -3591,19 +3440,16 @@
       <c r="V39">
         <v>20</v>
       </c>
-      <c r="W39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B40">
-        <v>30</v>
-      </c>
-      <c r="C40" t="s">
-        <v>141</v>
+      <c r="B40" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D40" s="12">
         <v>19</v>
@@ -3661,19 +3507,16 @@
       <c r="V40">
         <v>19</v>
       </c>
-      <c r="W40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B41">
-        <v>30</v>
-      </c>
-      <c r="C41" t="s">
-        <v>141</v>
+      <c r="B41" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D41" s="12">
         <v>18</v>
@@ -3728,19 +3571,16 @@
       <c r="V41">
         <v>-13</v>
       </c>
-      <c r="W41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B42">
-        <v>30</v>
-      </c>
-      <c r="C42" t="s">
-        <v>142</v>
+      <c r="B42" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D42" s="12">
         <v>19</v>
@@ -3798,19 +3638,16 @@
       <c r="V42">
         <v>12</v>
       </c>
-      <c r="W42" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B43">
-        <v>30</v>
-      </c>
-      <c r="C43" t="s">
-        <v>142</v>
+      <c r="B43" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D43" s="12">
         <v>18</v>
@@ -3865,19 +3702,16 @@
       <c r="V43">
         <v>-16</v>
       </c>
-      <c r="W43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B44">
-        <v>30</v>
-      </c>
-      <c r="C44" t="s">
-        <v>141</v>
+      <c r="B44" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D44" s="12">
         <v>22</v>
@@ -3935,19 +3769,16 @@
       <c r="V44">
         <v>32</v>
       </c>
-      <c r="W44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B45">
-        <v>30</v>
-      </c>
-      <c r="C45" t="s">
-        <v>137</v>
+      <c r="B45" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D45" s="12">
         <v>17</v>
@@ -3999,19 +3830,16 @@
       <c r="V45">
         <v>23</v>
       </c>
-      <c r="W45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B46">
-        <v>30</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
+      <c r="B46" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D46" s="12">
         <v>10</v>
@@ -4063,19 +3891,16 @@
       <c r="V46">
         <v>21</v>
       </c>
-      <c r="W46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B47">
-        <v>30</v>
-      </c>
-      <c r="C47" t="s">
-        <v>142</v>
+      <c r="B47" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D47" s="12">
         <v>18</v>
@@ -4127,19 +3952,16 @@
       <c r="V47">
         <v>-32</v>
       </c>
-      <c r="W47" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B48">
-        <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>138</v>
+      <c r="B48" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.52083333333333337</v>
       </c>
       <c r="D48" s="12">
         <v>24</v>
@@ -4194,19 +4016,16 @@
       <c r="V48">
         <v>19</v>
       </c>
-      <c r="W48" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B49">
-        <v>30</v>
-      </c>
-      <c r="C49" t="s">
-        <v>138</v>
+      <c r="B49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.52083333333333337</v>
       </c>
       <c r="D49" s="12">
         <v>18</v>
@@ -4261,19 +4080,16 @@
       <c r="V49">
         <v>32</v>
       </c>
-      <c r="W49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B50">
-        <v>30</v>
-      </c>
-      <c r="C50" t="s">
-        <v>136</v>
+      <c r="B50" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.41666666666666669</v>
       </c>
       <c r="D50" s="12">
         <v>15</v>
@@ -4331,19 +4147,16 @@
       <c r="V50">
         <v>6</v>
       </c>
-      <c r="W50" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B51">
-        <v>30</v>
-      </c>
-      <c r="C51" t="s">
-        <v>136</v>
+      <c r="B51" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.41666666666666669</v>
       </c>
       <c r="D51" s="12">
         <v>14</v>
@@ -4401,19 +4214,16 @@
       <c r="V51">
         <v>3</v>
       </c>
-      <c r="W51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B52">
-        <v>30</v>
-      </c>
-      <c r="C52" t="s">
-        <v>133</v>
+      <c r="B52" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.47916666666666669</v>
       </c>
       <c r="D52" s="12">
         <v>15</v>
@@ -4468,19 +4278,16 @@
       <c r="V52">
         <v>7</v>
       </c>
-      <c r="W52" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B53">
-        <v>30</v>
-      </c>
-      <c r="C53" t="s">
-        <v>133</v>
+      <c r="B53" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.47916666666666669</v>
       </c>
       <c r="D53" s="12">
         <v>14</v>
@@ -4535,19 +4342,16 @@
       <c r="V53">
         <v>4</v>
       </c>
-      <c r="W53" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B54">
-        <v>30</v>
-      </c>
-      <c r="C54" t="s">
-        <v>129</v>
+      <c r="B54" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.5</v>
       </c>
       <c r="D54" s="12">
         <v>18</v>
@@ -4599,19 +4403,16 @@
       <c r="V54">
         <v>34</v>
       </c>
-      <c r="W54" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B55">
-        <v>30</v>
-      </c>
-      <c r="C55" t="s">
-        <v>129</v>
+      <c r="B55" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.5</v>
       </c>
       <c r="D55" s="12">
         <v>24</v>
@@ -4663,19 +4464,16 @@
       <c r="V55">
         <v>24</v>
       </c>
-      <c r="W55" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B56">
-        <v>30</v>
-      </c>
-      <c r="C56" t="s">
-        <v>143</v>
+      <c r="B56" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.64583333333333337</v>
       </c>
       <c r="D56" s="12">
         <v>24</v>
@@ -4727,19 +4525,16 @@
       <c r="V56">
         <v>20</v>
       </c>
-      <c r="W56" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B57">
-        <v>30</v>
-      </c>
-      <c r="C57" t="s">
-        <v>143</v>
+      <c r="B57" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.64583333333333337</v>
       </c>
       <c r="D57" s="12">
         <v>18</v>
@@ -4791,19 +4586,16 @@
       <c r="V57">
         <v>34</v>
       </c>
-      <c r="W57" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B58">
-        <v>30</v>
-      </c>
-      <c r="C58" t="s">
-        <v>142</v>
+      <c r="B58" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D58" s="12">
         <v>22</v>
@@ -4855,19 +4647,16 @@
       <c r="V58">
         <v>-6</v>
       </c>
-      <c r="W58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B59">
-        <v>30</v>
-      </c>
-      <c r="C59" t="s">
-        <v>142</v>
+      <c r="B59" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D59" s="12">
         <v>28</v>
@@ -4919,19 +4708,16 @@
       <c r="V59">
         <v>0</v>
       </c>
-      <c r="W59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B60">
-        <v>30</v>
-      </c>
-      <c r="C60" t="s">
-        <v>143</v>
+      <c r="B60" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.64583333333333337</v>
       </c>
       <c r="D60" s="12">
         <v>12</v>
@@ -4983,11 +4769,11 @@
       <c r="V60">
         <v>-4</v>
       </c>
-      <c r="W60" t="s">
-        <v>131</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C24" r:id="rId1" display="1@:00" xr:uid="{2FFE11B1-0A19-D248-8D25-9235E2171C3F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>